<commit_message>
post-review 09/19, bonus not complete
</commit_message>
<xml_diff>
--- a/metro_budget_exercise.xlsx
+++ b/metro_budget_exercise.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sabri\Documents\NSS DA13\Excel\lookups-exercise-tosabrina\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42A6D08C-57B1-4560-A264-C466D4A0E9A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C64D9E33-27D6-452B-B2F8-8BD323925B16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40695" yWindow="0" windowWidth="12210" windowHeight="12885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metro_budget" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="93">
   <si>
     <t>Department</t>
   </si>
@@ -304,6 +304,15 @@
   </si>
   <si>
     <t>Actual spending amount - budget amount for fiscal year 2019</t>
+  </si>
+  <si>
+    <t>Question 3 - Bonus</t>
+  </si>
+  <si>
+    <t>Question 4 - Bonus</t>
+  </si>
+  <si>
+    <t>Question 5 - Bonus</t>
   </si>
 </sst>
 </file>
@@ -314,7 +323,7 @@
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -460,6 +469,13 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="34">
@@ -809,7 +825,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -822,6 +838,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="6"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1177,10 +1194,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P100"/>
+  <dimension ref="A1:P127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="B83" sqref="B83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1325,7 +1342,7 @@
         <v>-2.3069981751824741E-2</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F52" si="2">_xlfn.RANK.EQ(E3,$E:$E,1)</f>
+        <f>_xlfn.RANK.EQ(E3,$E:$E,1)</f>
         <v>22</v>
       </c>
       <c r="G3">
@@ -1335,15 +1352,15 @@
         <v>312433.70999999897</v>
       </c>
       <c r="I3">
-        <f t="shared" ref="I3:I52" si="3">H3-G3</f>
+        <f t="shared" ref="I3:I52" si="2">H3-G3</f>
         <v>-22366.290000001027</v>
       </c>
       <c r="J3" s="5">
-        <f t="shared" ref="J3:J52" si="4">IFERROR(I3/G3,0)</f>
+        <f t="shared" ref="J3:J52" si="3">IFERROR(I3/G3,0)</f>
         <v>-6.6804928315415249E-2</v>
       </c>
       <c r="K3">
-        <f t="shared" ref="K3:K52" si="5">RANK(J3,$J:$J,1)</f>
+        <f>RANK(J3,$J:$J,1)</f>
         <v>14</v>
       </c>
       <c r="L3">
@@ -1353,15 +1370,15 @@
         <v>322263.03999999998</v>
       </c>
       <c r="N3">
-        <f t="shared" ref="N3:N52" si="6">M3-L3</f>
+        <f t="shared" ref="N3:N52" si="4">M3-L3</f>
         <v>-436.96000000002095</v>
       </c>
       <c r="O3" s="5">
-        <f t="shared" ref="O3:O52" si="7">IFERROR(N3/L3,0)</f>
+        <f t="shared" ref="O3:O52" si="5">IFERROR(N3/L3,0)</f>
         <v>-1.3540749922529313E-3</v>
       </c>
       <c r="P3">
-        <f t="shared" ref="P3:P52" si="8">RANK(O3,$O:$O,1)</f>
+        <f>RANK(O3,$O:$O,1)</f>
         <v>37</v>
       </c>
     </row>
@@ -1384,7 +1401,7 @@
         <v>-4.9327413275443007E-3</v>
       </c>
       <c r="F4">
-        <f t="shared" si="2"/>
+        <f>_xlfn.RANK.EQ(E4,$E:$E,1)</f>
         <v>42</v>
       </c>
       <c r="G4">
@@ -1394,15 +1411,15 @@
         <v>3589693.2099999902</v>
       </c>
       <c r="I4">
+        <f t="shared" si="2"/>
+        <v>-62606.790000009816</v>
+      </c>
+      <c r="J4" s="5">
         <f t="shared" si="3"/>
-        <v>-62606.790000009816</v>
-      </c>
-      <c r="J4" s="5">
-        <f t="shared" si="4"/>
         <v>-1.7141743558856015E-2</v>
       </c>
       <c r="K4">
-        <f t="shared" si="5"/>
+        <f>RANK(J4,$J:$J,1)</f>
         <v>36</v>
       </c>
       <c r="L4">
@@ -1412,15 +1429,15 @@
         <v>3564983.04999999</v>
       </c>
       <c r="N4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>-97416.950000009965</v>
       </c>
       <c r="O4" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>-2.6599210899959033E-2</v>
       </c>
       <c r="P4">
-        <f t="shared" si="8"/>
+        <f>RANK(O4,$O:$O,1)</f>
         <v>25</v>
       </c>
     </row>
@@ -1443,7 +1460,7 @@
         <v>-9.4273968477453174E-2</v>
       </c>
       <c r="F5">
-        <f t="shared" si="2"/>
+        <f>_xlfn.RANK.EQ(E5,$E:$E,1)</f>
         <v>4</v>
       </c>
       <c r="G5">
@@ -1453,15 +1470,15 @@
         <v>7020609.3200000003</v>
       </c>
       <c r="I5">
+        <f t="shared" si="2"/>
+        <v>-947690.6799999997</v>
+      </c>
+      <c r="J5" s="5">
         <f t="shared" si="3"/>
-        <v>-947690.6799999997</v>
-      </c>
-      <c r="J5" s="5">
-        <f t="shared" si="4"/>
         <v>-0.118932605449092</v>
       </c>
       <c r="K5">
-        <f t="shared" si="5"/>
+        <f>RANK(J5,$J:$J,1)</f>
         <v>5</v>
       </c>
       <c r="L5">
@@ -1471,15 +1488,15 @@
         <v>7497322.9100000001</v>
       </c>
       <c r="N5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>-262277.08999999985</v>
       </c>
       <c r="O5" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>-3.3800336357544182E-2</v>
       </c>
       <c r="P5">
-        <f t="shared" si="8"/>
+        <f>RANK(O5,$O:$O,1)</f>
         <v>22</v>
       </c>
     </row>
@@ -1502,7 +1519,7 @@
         <v>-5.7149963352064452E-2</v>
       </c>
       <c r="F6">
-        <f t="shared" si="2"/>
+        <f>_xlfn.RANK.EQ(E6,$E:$E,1)</f>
         <v>11</v>
       </c>
       <c r="G6">
@@ -1512,15 +1529,15 @@
         <v>427758.64</v>
       </c>
       <c r="I6">
+        <f t="shared" si="2"/>
+        <v>-741.35999999998603</v>
+      </c>
+      <c r="J6" s="5">
         <f t="shared" si="3"/>
-        <v>-741.35999999998603</v>
-      </c>
-      <c r="J6" s="5">
-        <f t="shared" si="4"/>
         <v>-1.7301283547257551E-3</v>
       </c>
       <c r="K6">
-        <f t="shared" si="5"/>
+        <f>RANK(J6,$J:$J,1)</f>
         <v>44</v>
       </c>
       <c r="L6">
@@ -1530,15 +1547,15 @@
         <v>445114.28999999899</v>
       </c>
       <c r="N6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>-85.710000001010485</v>
       </c>
       <c r="O6" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>-1.925202156356929E-4</v>
       </c>
       <c r="P6">
-        <f t="shared" si="8"/>
+        <f>RANK(O6,$O:$O,1)</f>
         <v>39</v>
       </c>
     </row>
@@ -1561,7 +1578,7 @@
         <v>-0.11502817362571344</v>
       </c>
       <c r="F7">
-        <f t="shared" si="2"/>
+        <f>_xlfn.RANK.EQ(E7,$E:$E,1)</f>
         <v>2</v>
       </c>
       <c r="G7">
@@ -1571,15 +1588,15 @@
         <v>3051483.41</v>
       </c>
       <c r="I7">
+        <f t="shared" si="2"/>
+        <v>-339416.58999999985</v>
+      </c>
+      <c r="J7" s="5">
         <f t="shared" si="3"/>
-        <v>-339416.58999999985</v>
-      </c>
-      <c r="J7" s="5">
-        <f t="shared" si="4"/>
         <v>-0.10009631366303927</v>
       </c>
       <c r="K7">
-        <f t="shared" si="5"/>
+        <f>RANK(J7,$J:$J,1)</f>
         <v>8</v>
       </c>
       <c r="L7">
@@ -1589,15 +1606,15 @@
         <v>2946440.08</v>
       </c>
       <c r="N7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>-398759.91999999993</v>
       </c>
       <c r="O7" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>-0.11920361114432618</v>
       </c>
       <c r="P7">
-        <f t="shared" si="8"/>
+        <f>RANK(O7,$O:$O,1)</f>
         <v>4</v>
       </c>
     </row>
@@ -1620,7 +1637,7 @@
         <v>-0.15235918433091292</v>
       </c>
       <c r="F8" s="9">
-        <f t="shared" si="2"/>
+        <f>_xlfn.RANK.EQ(E8,$E:$E,1)</f>
         <v>1</v>
       </c>
       <c r="G8">
@@ -1630,15 +1647,15 @@
         <v>1383905.98999999</v>
       </c>
       <c r="I8">
+        <f t="shared" si="2"/>
+        <v>-206794.01000001002</v>
+      </c>
+      <c r="J8" s="5">
         <f t="shared" si="3"/>
-        <v>-206794.01000001002</v>
-      </c>
-      <c r="J8" s="5">
-        <f t="shared" si="4"/>
         <v>-0.13000189224870184</v>
       </c>
       <c r="K8">
-        <f t="shared" si="5"/>
+        <f>RANK(J8,$J:$J,1)</f>
         <v>4</v>
       </c>
       <c r="L8">
@@ -1648,15 +1665,15 @@
         <v>1337735.3199999901</v>
       </c>
       <c r="N8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>-241564.68000000995</v>
       </c>
       <c r="O8" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>-0.15295680364719175</v>
       </c>
       <c r="P8">
-        <f t="shared" si="8"/>
+        <f>RANK(O8,$O:$O,1)</f>
         <v>2</v>
       </c>
     </row>
@@ -1679,7 +1696,7 @@
         <v>-4.2417130511048909E-2</v>
       </c>
       <c r="F9">
-        <f t="shared" si="2"/>
+        <f>_xlfn.RANK.EQ(E9,$E:$E,1)</f>
         <v>16</v>
       </c>
       <c r="G9">
@@ -1689,15 +1706,15 @@
         <v>9929059.5199999996</v>
       </c>
       <c r="I9">
+        <f t="shared" si="2"/>
+        <v>-1144640.4800000004</v>
+      </c>
+      <c r="J9" s="5">
         <f t="shared" si="3"/>
-        <v>-1144640.4800000004</v>
-      </c>
-      <c r="J9" s="5">
-        <f t="shared" si="4"/>
         <v>-0.10336567542917005</v>
       </c>
       <c r="K9">
-        <f t="shared" si="5"/>
+        <f>RANK(J9,$J:$J,1)</f>
         <v>7</v>
       </c>
       <c r="L9">
@@ -1707,15 +1724,15 @@
         <v>9993599.52999999</v>
       </c>
       <c r="N9">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>-796900.47000000998</v>
       </c>
       <c r="O9" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>-7.3852043000788653E-2</v>
       </c>
       <c r="P9">
-        <f t="shared" si="8"/>
+        <f>RANK(O9,$O:$O,1)</f>
         <v>9</v>
       </c>
     </row>
@@ -1738,7 +1755,7 @@
         <v>-8.1681998646514792E-2</v>
       </c>
       <c r="F10">
-        <f t="shared" si="2"/>
+        <f>_xlfn.RANK.EQ(E10,$E:$E,1)</f>
         <v>6</v>
       </c>
       <c r="G10">
@@ -1748,15 +1765,15 @@
         <v>467907.84000000003</v>
       </c>
       <c r="I10">
+        <f t="shared" si="2"/>
+        <v>-27292.159999999974</v>
+      </c>
+      <c r="J10" s="5">
         <f t="shared" si="3"/>
-        <v>-27292.159999999974</v>
-      </c>
-      <c r="J10" s="5">
-        <f t="shared" si="4"/>
         <v>-5.5113408723747932E-2</v>
       </c>
       <c r="K10">
-        <f t="shared" si="5"/>
+        <f>RANK(J10,$J:$J,1)</f>
         <v>17</v>
       </c>
       <c r="L10">
@@ -1766,15 +1783,15 @@
         <v>478318.92</v>
       </c>
       <c r="N10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>-9181.0800000000163</v>
       </c>
       <c r="O10" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>-1.883298461538465E-2</v>
       </c>
       <c r="P10">
-        <f t="shared" si="8"/>
+        <f>RANK(O10,$O:$O,1)</f>
         <v>29</v>
       </c>
     </row>
@@ -1797,25 +1814,25 @@
         <v>0</v>
       </c>
       <c r="F11">
+        <f>_xlfn.RANK.EQ(E11,$E:$E,1)</f>
+        <v>47</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
         <f t="shared" si="2"/>
-        <v>47</v>
-      </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
-      <c r="H11">
-        <v>0</v>
-      </c>
-      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11" s="5">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J11" s="5">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
       <c r="K11">
-        <f t="shared" si="5"/>
+        <f>RANK(J11,$J:$J,1)</f>
         <v>48</v>
       </c>
       <c r="L11">
@@ -1825,15 +1842,15 @@
         <v>63771.91</v>
       </c>
       <c r="N11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>-311228.08999999997</v>
       </c>
       <c r="O11" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>-0.82994157333333329</v>
       </c>
       <c r="P11">
-        <f t="shared" si="8"/>
+        <f>RANK(O11,$O:$O,1)</f>
         <v>1</v>
       </c>
     </row>
@@ -1856,7 +1873,7 @@
         <v>-5.0060657805601608E-2</v>
       </c>
       <c r="F12">
-        <f t="shared" si="2"/>
+        <f>_xlfn.RANK.EQ(E12,$E:$E,1)</f>
         <v>13</v>
       </c>
       <c r="G12">
@@ -1866,15 +1883,15 @@
         <v>4205555.5999999996</v>
       </c>
       <c r="I12">
+        <f t="shared" si="2"/>
+        <v>-494844.40000000037</v>
+      </c>
+      <c r="J12" s="5">
         <f t="shared" si="3"/>
-        <v>-494844.40000000037</v>
-      </c>
-      <c r="J12" s="5">
-        <f t="shared" si="4"/>
         <v>-0.10527708280146378</v>
       </c>
       <c r="K12">
-        <f t="shared" si="5"/>
+        <f>RANK(J12,$J:$J,1)</f>
         <v>6</v>
       </c>
       <c r="L12">
@@ -1884,15 +1901,15 @@
         <v>4371713.1399999997</v>
       </c>
       <c r="N12">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>-306086.86000000034</v>
       </c>
       <c r="O12" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>-6.5433934755654441E-2</v>
       </c>
       <c r="P12">
-        <f t="shared" si="8"/>
+        <f>RANK(O12,$O:$O,1)</f>
         <v>10</v>
       </c>
     </row>
@@ -1915,7 +1932,7 @@
         <v>-1.2912833886247806E-2</v>
       </c>
       <c r="F13">
-        <f t="shared" si="2"/>
+        <f>_xlfn.RANK.EQ(E13,$E:$E,1)</f>
         <v>33</v>
       </c>
       <c r="G13">
@@ -1925,15 +1942,15 @@
         <v>5909077.9399999902</v>
       </c>
       <c r="I13">
+        <f t="shared" si="2"/>
+        <v>-314622.06000000983</v>
+      </c>
+      <c r="J13" s="5">
         <f t="shared" si="3"/>
-        <v>-314622.06000000983</v>
-      </c>
-      <c r="J13" s="5">
-        <f t="shared" si="4"/>
         <v>-5.0552253482656594E-2</v>
       </c>
       <c r="K13">
-        <f t="shared" si="5"/>
+        <f>RANK(J13,$J:$J,1)</f>
         <v>18</v>
       </c>
       <c r="L13">
@@ -1943,15 +1960,15 @@
         <v>6056976.6699999999</v>
       </c>
       <c r="N13">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>-150323.33000000007</v>
       </c>
       <c r="O13" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>-2.4217184605222895E-2</v>
       </c>
       <c r="P13">
-        <f t="shared" si="8"/>
+        <f>RANK(O13,$O:$O,1)</f>
         <v>27</v>
       </c>
     </row>
@@ -1974,7 +1991,7 @@
         <v>-1.3637949218750009E-2</v>
       </c>
       <c r="F14">
-        <f t="shared" si="2"/>
+        <f>_xlfn.RANK.EQ(E14,$E:$E,1)</f>
         <v>30</v>
       </c>
       <c r="G14">
@@ -1984,15 +2001,15 @@
         <v>524402.98</v>
       </c>
       <c r="I14">
+        <f t="shared" si="2"/>
+        <v>-6097.0200000000186</v>
+      </c>
+      <c r="J14" s="5">
         <f t="shared" si="3"/>
-        <v>-6097.0200000000186</v>
-      </c>
-      <c r="J14" s="5">
-        <f t="shared" si="4"/>
         <v>-1.1492968897266765E-2</v>
       </c>
       <c r="K14">
-        <f t="shared" si="5"/>
+        <f>RANK(J14,$J:$J,1)</f>
         <v>40</v>
       </c>
       <c r="L14">
@@ -2002,15 +2019,15 @@
         <v>504989.88</v>
       </c>
       <c r="N14">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>-21210.119999999995</v>
       </c>
       <c r="O14" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>-4.0308095781071827E-2</v>
       </c>
       <c r="P14">
-        <f t="shared" si="8"/>
+        <f>RANK(O14,$O:$O,1)</f>
         <v>19</v>
       </c>
     </row>
@@ -2033,7 +2050,7 @@
         <v>3.1837408866824991E-3</v>
       </c>
       <c r="F15">
-        <f t="shared" si="2"/>
+        <f>_xlfn.RANK.EQ(E15,$E:$E,1)</f>
         <v>51</v>
       </c>
       <c r="G15">
@@ -2043,15 +2060,15 @@
         <v>175966389.24999899</v>
       </c>
       <c r="I15">
+        <f t="shared" si="2"/>
+        <v>-8201410.7500010133</v>
+      </c>
+      <c r="J15" s="5">
         <f t="shared" si="3"/>
-        <v>-8201410.7500010133</v>
-      </c>
-      <c r="J15" s="5">
-        <f t="shared" si="4"/>
         <v>-4.4532273014072019E-2</v>
       </c>
       <c r="K15">
-        <f t="shared" si="5"/>
+        <f>RANK(J15,$J:$J,1)</f>
         <v>24</v>
       </c>
       <c r="L15">
@@ -2061,15 +2078,15 @@
         <v>184450910.84999901</v>
       </c>
       <c r="N15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>-4502589.1500009894</v>
       </c>
       <c r="O15" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>-2.3829085727446114E-2</v>
       </c>
       <c r="P15">
-        <f t="shared" si="8"/>
+        <f>RANK(O15,$O:$O,1)</f>
         <v>28</v>
       </c>
     </row>
@@ -2092,7 +2109,7 @@
         <v>-1.1850188616360429E-2</v>
       </c>
       <c r="F16">
-        <f t="shared" si="2"/>
+        <f>_xlfn.RANK.EQ(E16,$E:$E,1)</f>
         <v>37</v>
       </c>
       <c r="G16">
@@ -2102,15 +2119,15 @@
         <v>7350464.0800000001</v>
       </c>
       <c r="I16">
+        <f t="shared" si="2"/>
+        <v>-2035.9199999999255</v>
+      </c>
+      <c r="J16" s="5">
         <f t="shared" si="3"/>
-        <v>-2035.9199999999255</v>
-      </c>
-      <c r="J16" s="5">
-        <f t="shared" si="4"/>
         <v>-2.769017341040361E-4</v>
       </c>
       <c r="K16">
-        <f t="shared" si="5"/>
+        <f>RANK(J16,$J:$J,1)</f>
         <v>46</v>
       </c>
       <c r="L16">
@@ -2120,15 +2137,15 @@
         <v>7397093</v>
       </c>
       <c r="N16">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>-107</v>
       </c>
       <c r="O16" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>-1.4464932677229222E-5</v>
       </c>
       <c r="P16">
-        <f t="shared" si="8"/>
+        <f>RANK(O16,$O:$O,1)</f>
         <v>43</v>
       </c>
     </row>
@@ -2151,7 +2168,7 @@
         <v>-2.8351094826658003E-2</v>
       </c>
       <c r="F17">
-        <f t="shared" si="2"/>
+        <f>_xlfn.RANK.EQ(E17,$E:$E,1)</f>
         <v>21</v>
       </c>
       <c r="G17">
@@ -2161,15 +2178,15 @@
         <v>14645233.51</v>
       </c>
       <c r="I17">
+        <f t="shared" si="2"/>
+        <v>-664466.49000000022</v>
+      </c>
+      <c r="J17" s="5">
         <f t="shared" si="3"/>
-        <v>-664466.49000000022</v>
-      </c>
-      <c r="J17" s="5">
-        <f t="shared" si="4"/>
         <v>-4.3401666263871937E-2</v>
       </c>
       <c r="K17">
-        <f t="shared" si="5"/>
+        <f>RANK(J17,$J:$J,1)</f>
         <v>25</v>
       </c>
       <c r="L17">
@@ -2179,15 +2196,15 @@
         <v>14346057.039999999</v>
       </c>
       <c r="N17">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>-965742.96000000089</v>
       </c>
       <c r="O17" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>-6.3071811282801551E-2</v>
       </c>
       <c r="P17">
-        <f t="shared" si="8"/>
+        <f>RANK(O17,$O:$O,1)</f>
         <v>11</v>
       </c>
     </row>
@@ -2210,7 +2227,7 @@
         <v>-5.4037002206391245E-2</v>
       </c>
       <c r="F18">
-        <f t="shared" si="2"/>
+        <f>_xlfn.RANK.EQ(E18,$E:$E,1)</f>
         <v>12</v>
       </c>
       <c r="G18">
@@ -2220,15 +2237,15 @@
         <v>2671745.94</v>
       </c>
       <c r="I18">
+        <f t="shared" si="2"/>
+        <v>-189254.06000000006</v>
+      </c>
+      <c r="J18" s="5">
         <f t="shared" si="3"/>
-        <v>-189254.06000000006</v>
-      </c>
-      <c r="J18" s="5">
-        <f t="shared" si="4"/>
         <v>-6.6149619014330668E-2</v>
       </c>
       <c r="K18">
-        <f t="shared" si="5"/>
+        <f>RANK(J18,$J:$J,1)</f>
         <v>15</v>
       </c>
       <c r="L18">
@@ -2238,15 +2255,15 @@
         <v>2535637.09</v>
       </c>
       <c r="N18">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>-374962.91000000015</v>
       </c>
       <c r="O18" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>-0.12882667147667154</v>
       </c>
       <c r="P18">
-        <f t="shared" si="8"/>
+        <f>RANK(O18,$O:$O,1)</f>
         <v>3</v>
       </c>
     </row>
@@ -2269,7 +2286,7 @@
         <v>-4.258504294298146E-2</v>
       </c>
       <c r="F19">
-        <f t="shared" si="2"/>
+        <f>_xlfn.RANK.EQ(E19,$E:$E,1)</f>
         <v>15</v>
       </c>
       <c r="G19">
@@ -2279,15 +2296,15 @@
         <v>8991707.2399999909</v>
       </c>
       <c r="I19">
+        <f t="shared" si="2"/>
+        <v>-721592.76000000909</v>
+      </c>
+      <c r="J19" s="5">
         <f t="shared" si="3"/>
-        <v>-721592.76000000909</v>
-      </c>
-      <c r="J19" s="5">
-        <f t="shared" si="4"/>
         <v>-7.4289145810384635E-2</v>
       </c>
       <c r="K19">
-        <f t="shared" si="5"/>
+        <f>RANK(J19,$J:$J,1)</f>
         <v>12</v>
       </c>
       <c r="L19">
@@ -2297,15 +2314,15 @@
         <v>8766655.9100000001</v>
       </c>
       <c r="N19">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>-576344.08999999985</v>
       </c>
       <c r="O19" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>-6.1687262121374278E-2</v>
       </c>
       <c r="P19">
-        <f t="shared" si="8"/>
+        <f>RANK(O19,$O:$O,1)</f>
         <v>12</v>
       </c>
     </row>
@@ -2328,7 +2345,7 @@
         <v>-1.2379538203300809E-5</v>
       </c>
       <c r="F20">
-        <f t="shared" si="2"/>
+        <f>_xlfn.RANK.EQ(E20,$E:$E,1)</f>
         <v>46</v>
       </c>
       <c r="G20">
@@ -2338,15 +2355,15 @@
         <v>131839624.37</v>
       </c>
       <c r="I20">
+        <f t="shared" si="2"/>
+        <v>-9775.6299999952316</v>
+      </c>
+      <c r="J20" s="5">
         <f t="shared" si="3"/>
-        <v>-9775.6299999952316</v>
-      </c>
-      <c r="J20" s="5">
-        <f t="shared" si="4"/>
         <v>-7.4142392760188761E-5</v>
       </c>
       <c r="K20">
-        <f t="shared" si="5"/>
+        <f>RANK(J20,$J:$J,1)</f>
         <v>47</v>
       </c>
       <c r="L20">
@@ -2356,15 +2373,15 @@
         <v>130621283.53999899</v>
       </c>
       <c r="N20">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>-116.46000100672245</v>
       </c>
       <c r="O20" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>-8.9158438821450736E-7</v>
       </c>
       <c r="P20">
-        <f t="shared" si="8"/>
+        <f>RANK(O20,$O:$O,1)</f>
         <v>46</v>
       </c>
     </row>
@@ -2387,7 +2404,7 @@
         <v>-7.9052463618023094E-2</v>
       </c>
       <c r="F21">
-        <f t="shared" si="2"/>
+        <f>_xlfn.RANK.EQ(E21,$E:$E,1)</f>
         <v>9</v>
       </c>
       <c r="G21">
@@ -2397,15 +2414,15 @@
         <v>22655993.629999999</v>
       </c>
       <c r="I21">
+        <f t="shared" si="2"/>
+        <v>-1841406.370000001</v>
+      </c>
+      <c r="J21" s="5">
         <f t="shared" si="3"/>
-        <v>-1841406.370000001</v>
-      </c>
-      <c r="J21" s="5">
-        <f t="shared" si="4"/>
         <v>-7.5167420624229556E-2</v>
       </c>
       <c r="K21">
-        <f t="shared" si="5"/>
+        <f>RANK(J21,$J:$J,1)</f>
         <v>11</v>
       </c>
       <c r="L21">
@@ -2415,15 +2432,15 @@
         <v>23434073.089999899</v>
       </c>
       <c r="N21">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>-888926.91000010073</v>
       </c>
       <c r="O21" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>-3.6546762734864152E-2</v>
       </c>
       <c r="P21">
-        <f t="shared" si="8"/>
+        <f>RANK(O21,$O:$O,1)</f>
         <v>21</v>
       </c>
     </row>
@@ -2446,7 +2463,7 @@
         <v>-1.3285502334437123E-2</v>
       </c>
       <c r="F22">
-        <f t="shared" si="2"/>
+        <f>_xlfn.RANK.EQ(E22,$E:$E,1)</f>
         <v>32</v>
       </c>
       <c r="G22">
@@ -2456,15 +2473,15 @@
         <v>11791977.9699999</v>
       </c>
       <c r="I22">
+        <f t="shared" si="2"/>
+        <v>-188722.03000009991</v>
+      </c>
+      <c r="J22" s="5">
         <f t="shared" si="3"/>
-        <v>-188722.03000009991</v>
-      </c>
-      <c r="J22" s="5">
-        <f t="shared" si="4"/>
         <v>-1.5752170574348738E-2</v>
       </c>
       <c r="K22">
-        <f t="shared" si="5"/>
+        <f>RANK(J22,$J:$J,1)</f>
         <v>38</v>
       </c>
       <c r="L22">
@@ -2474,15 +2491,15 @@
         <v>11934454.77</v>
       </c>
       <c r="N22">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>-745.23000000044703</v>
       </c>
       <c r="O22" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>-6.2439674240938325E-5</v>
       </c>
       <c r="P22">
-        <f t="shared" si="8"/>
+        <f>RANK(O22,$O:$O,1)</f>
         <v>42</v>
       </c>
     </row>
@@ -2505,7 +2522,7 @@
         <v>-3.9590110100806722E-2</v>
       </c>
       <c r="F23">
-        <f t="shared" si="2"/>
+        <f>_xlfn.RANK.EQ(E23,$E:$E,1)</f>
         <v>18</v>
       </c>
       <c r="G23">
@@ -2515,15 +2532,15 @@
         <v>21722126.219999898</v>
       </c>
       <c r="I23">
+        <f t="shared" si="2"/>
+        <v>-961673.78000010177</v>
+      </c>
+      <c r="J23" s="5">
         <f t="shared" si="3"/>
-        <v>-961673.78000010177</v>
-      </c>
-      <c r="J23" s="5">
-        <f t="shared" si="4"/>
         <v>-4.2394738976719144E-2</v>
       </c>
       <c r="K23">
-        <f t="shared" si="5"/>
+        <f>RANK(J23,$J:$J,1)</f>
         <v>26</v>
       </c>
       <c r="L23">
@@ -2533,15 +2550,15 @@
         <v>22619057.440000001</v>
       </c>
       <c r="N23">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>-601242.55999999866</v>
       </c>
       <c r="O23" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>-2.5892971236375011E-2</v>
       </c>
       <c r="P23">
-        <f t="shared" si="8"/>
+        <f>RANK(O23,$O:$O,1)</f>
         <v>26</v>
       </c>
     </row>
@@ -2564,7 +2581,7 @@
         <v>-1.3334943305713101E-2</v>
       </c>
       <c r="F24">
-        <f t="shared" si="2"/>
+        <f>_xlfn.RANK.EQ(E24,$E:$E,1)</f>
         <v>31</v>
       </c>
       <c r="G24">
@@ -2574,15 +2591,15 @@
         <v>1067214.42</v>
       </c>
       <c r="I24">
+        <f t="shared" si="2"/>
+        <v>-45485.580000000075</v>
+      </c>
+      <c r="J24" s="5">
         <f t="shared" si="3"/>
-        <v>-45485.580000000075</v>
-      </c>
-      <c r="J24" s="5">
-        <f t="shared" si="4"/>
         <v>-4.087856565111897E-2</v>
       </c>
       <c r="K24">
-        <f t="shared" si="5"/>
+        <f>RANK(J24,$J:$J,1)</f>
         <v>28</v>
       </c>
       <c r="L24">
@@ -2592,15 +2609,15 @@
         <v>1112527.1200000001</v>
       </c>
       <c r="N24">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>-72.879999999888241</v>
       </c>
       <c r="O24" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>-6.5504224339284781E-5</v>
       </c>
       <c r="P24">
-        <f t="shared" si="8"/>
+        <f>RANK(O24,$O:$O,1)</f>
         <v>41</v>
       </c>
     </row>
@@ -2623,7 +2640,7 @@
         <v>-1.0226130964676661E-2</v>
       </c>
       <c r="F25">
-        <f t="shared" si="2"/>
+        <f>_xlfn.RANK.EQ(E25,$E:$E,1)</f>
         <v>38</v>
       </c>
       <c r="G25">
@@ -2633,15 +2650,15 @@
         <v>497194.20999999897</v>
       </c>
       <c r="I25">
+        <f t="shared" si="2"/>
+        <v>-8005.7900000010268</v>
+      </c>
+      <c r="J25" s="5">
         <f t="shared" si="3"/>
-        <v>-8005.7900000010268</v>
-      </c>
-      <c r="J25" s="5">
-        <f t="shared" si="4"/>
         <v>-1.5846773555029746E-2</v>
       </c>
       <c r="K25">
-        <f t="shared" si="5"/>
+        <f>RANK(J25,$J:$J,1)</f>
         <v>37</v>
       </c>
       <c r="L25">
@@ -2651,15 +2668,15 @@
         <v>494775.1</v>
       </c>
       <c r="N25">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>-1724.9000000000233</v>
       </c>
       <c r="O25" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>-3.4741188318228064E-3</v>
       </c>
       <c r="P25">
-        <f t="shared" si="8"/>
+        <f>RANK(O25,$O:$O,1)</f>
         <v>35</v>
       </c>
     </row>
@@ -2682,7 +2699,7 @@
         <v>-8.5306091660634673E-2</v>
       </c>
       <c r="F26">
-        <f t="shared" si="2"/>
+        <f>_xlfn.RANK.EQ(E26,$E:$E,1)</f>
         <v>5</v>
       </c>
       <c r="G26">
@@ -2692,15 +2709,15 @@
         <v>5122329.02999999</v>
       </c>
       <c r="I26">
+        <f t="shared" si="2"/>
+        <v>-319870.97000000998</v>
+      </c>
+      <c r="J26" s="5">
         <f t="shared" si="3"/>
-        <v>-319870.97000000998</v>
-      </c>
-      <c r="J26" s="5">
-        <f t="shared" si="4"/>
         <v>-5.8776040939327839E-2</v>
       </c>
       <c r="K26">
-        <f t="shared" si="5"/>
+        <f>RANK(J26,$J:$J,1)</f>
         <v>16</v>
       </c>
       <c r="L26">
@@ -2710,15 +2727,15 @@
         <v>5117235.21</v>
       </c>
       <c r="N26">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>-313464.79000000004</v>
       </c>
       <c r="O26" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>-5.7720881286022069E-2</v>
       </c>
       <c r="P26">
-        <f t="shared" si="8"/>
+        <f>RANK(O26,$O:$O,1)</f>
         <v>13</v>
       </c>
     </row>
@@ -2741,43 +2758,43 @@
         <v>0</v>
       </c>
       <c r="F27">
+        <f>_xlfn.RANK.EQ(E27,$E:$E,1)</f>
+        <v>47</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27">
         <f t="shared" si="2"/>
-        <v>47</v>
-      </c>
-      <c r="G27">
-        <v>0</v>
-      </c>
-      <c r="H27">
-        <v>0</v>
-      </c>
-      <c r="I27">
+        <v>0</v>
+      </c>
+      <c r="J27" s="5">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J27" s="5">
+      <c r="K27">
+        <f>RANK(J27,$J:$J,1)</f>
+        <v>48</v>
+      </c>
+      <c r="L27">
+        <v>0</v>
+      </c>
+      <c r="M27">
+        <v>0</v>
+      </c>
+      <c r="N27">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="K27">
+      <c r="O27" s="5">
         <f t="shared" si="5"/>
-        <v>48</v>
-      </c>
-      <c r="L27">
-        <v>0</v>
-      </c>
-      <c r="M27">
-        <v>0</v>
-      </c>
-      <c r="N27">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="O27" s="5">
-        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="P27">
-        <f t="shared" si="8"/>
+        <f>RANK(O27,$O:$O,1)</f>
         <v>48</v>
       </c>
     </row>
@@ -2800,7 +2817,7 @@
         <v>-9.5782760864849215E-2</v>
       </c>
       <c r="F28">
-        <f t="shared" si="2"/>
+        <f>_xlfn.RANK.EQ(E28,$E:$E,1)</f>
         <v>3</v>
       </c>
       <c r="G28">
@@ -2810,15 +2827,15 @@
         <v>1281335.23</v>
       </c>
       <c r="I28">
+        <f t="shared" si="2"/>
+        <v>-264364.77</v>
+      </c>
+      <c r="J28" s="5">
         <f t="shared" si="3"/>
-        <v>-264364.77</v>
-      </c>
-      <c r="J28" s="5">
-        <f t="shared" si="4"/>
         <v>-0.17103239309050916</v>
       </c>
       <c r="K28">
-        <f t="shared" si="5"/>
+        <f>RANK(J28,$J:$J,1)</f>
         <v>2</v>
       </c>
       <c r="L28">
@@ -2828,15 +2845,15 @@
         <v>1393285.06</v>
       </c>
       <c r="N28">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>-132614.93999999994</v>
       </c>
       <c r="O28" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>-8.6909325643882263E-2</v>
       </c>
       <c r="P28">
-        <f t="shared" si="8"/>
+        <f>RANK(O28,$O:$O,1)</f>
         <v>7</v>
       </c>
     </row>
@@ -2859,7 +2876,7 @@
         <v>-1.4800253727847622E-2</v>
       </c>
       <c r="F29">
-        <f t="shared" si="2"/>
+        <f>_xlfn.RANK.EQ(E29,$E:$E,1)</f>
         <v>28</v>
       </c>
       <c r="G29">
@@ -2869,15 +2886,15 @@
         <v>2665264.4399999902</v>
       </c>
       <c r="I29">
+        <f t="shared" si="2"/>
+        <v>-114235.56000000983</v>
+      </c>
+      <c r="J29" s="5">
         <f t="shared" si="3"/>
-        <v>-114235.56000000983</v>
-      </c>
-      <c r="J29" s="5">
-        <f t="shared" si="4"/>
         <v>-4.1099320021590155E-2</v>
       </c>
       <c r="K29">
-        <f t="shared" si="5"/>
+        <f>RANK(J29,$J:$J,1)</f>
         <v>27</v>
       </c>
       <c r="L29">
@@ -2887,15 +2904,15 @@
         <v>2889864.67</v>
       </c>
       <c r="N29">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>-35.330000000074506</v>
       </c>
       <c r="O29" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>-1.2225336516860273E-5</v>
       </c>
       <c r="P29">
-        <f t="shared" si="8"/>
+        <f>RANK(O29,$O:$O,1)</f>
         <v>44</v>
       </c>
     </row>
@@ -2918,7 +2935,7 @@
         <v>-8.3831374359143746E-3</v>
       </c>
       <c r="F30">
-        <f t="shared" si="2"/>
+        <f>_xlfn.RANK.EQ(E30,$E:$E,1)</f>
         <v>40</v>
       </c>
       <c r="G30">
@@ -2928,15 +2945,15 @@
         <v>12685514.279999901</v>
       </c>
       <c r="I30">
+        <f t="shared" si="2"/>
+        <v>-50385.720000099391</v>
+      </c>
+      <c r="J30" s="5">
         <f t="shared" si="3"/>
-        <v>-50385.720000099391</v>
-      </c>
-      <c r="J30" s="5">
-        <f t="shared" si="4"/>
         <v>-3.9561962641116366E-3</v>
       </c>
       <c r="K30">
-        <f t="shared" si="5"/>
+        <f>RANK(J30,$J:$J,1)</f>
         <v>42</v>
       </c>
       <c r="L30">
@@ -2946,15 +2963,15 @@
         <v>12826009.609999999</v>
       </c>
       <c r="N30">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>-35290.390000000596</v>
       </c>
       <c r="O30" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>-2.7439209100169185E-3</v>
       </c>
       <c r="P30">
-        <f t="shared" si="8"/>
+        <f>RANK(O30,$O:$O,1)</f>
         <v>36</v>
       </c>
     </row>
@@ -2977,7 +2994,7 @@
         <v>-1.4030533529678329E-2</v>
       </c>
       <c r="F31">
-        <f t="shared" si="2"/>
+        <f>_xlfn.RANK.EQ(E31,$E:$E,1)</f>
         <v>29</v>
       </c>
       <c r="G31">
@@ -2987,15 +3004,15 @@
         <v>1762676.85</v>
       </c>
       <c r="I31">
+        <f t="shared" si="2"/>
+        <v>-60623.149999999907</v>
+      </c>
+      <c r="J31" s="5">
         <f t="shared" si="3"/>
-        <v>-60623.149999999907</v>
-      </c>
-      <c r="J31" s="5">
-        <f t="shared" si="4"/>
         <v>-3.3249136181648611E-2</v>
       </c>
       <c r="K31">
-        <f t="shared" si="5"/>
+        <f>RANK(J31,$J:$J,1)</f>
         <v>32</v>
       </c>
       <c r="L31">
@@ -3005,15 +3022,15 @@
         <v>1801391.34</v>
       </c>
       <c r="N31">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>-69308.659999999916</v>
       </c>
       <c r="O31" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>-3.7049585716576634E-2</v>
       </c>
       <c r="P31">
-        <f t="shared" si="8"/>
+        <f>RANK(O31,$O:$O,1)</f>
         <v>20</v>
       </c>
     </row>
@@ -3036,7 +3053,7 @@
         <v>-1.2294942827617691E-2</v>
       </c>
       <c r="F32">
-        <f t="shared" si="2"/>
+        <f>_xlfn.RANK.EQ(E32,$E:$E,1)</f>
         <v>36</v>
       </c>
       <c r="G32">
@@ -3046,15 +3063,15 @@
         <v>6084985.4699999997</v>
       </c>
       <c r="I32">
+        <f t="shared" si="2"/>
+        <v>-110514.53000000026</v>
+      </c>
+      <c r="J32" s="5">
         <f t="shared" si="3"/>
-        <v>-110514.53000000026</v>
-      </c>
-      <c r="J32" s="5">
-        <f t="shared" si="4"/>
         <v>-1.7837871035428981E-2</v>
       </c>
       <c r="K32">
-        <f t="shared" si="5"/>
+        <f>RANK(J32,$J:$J,1)</f>
         <v>35</v>
       </c>
       <c r="L32">
@@ -3064,15 +3081,15 @@
         <v>5987572.0199999996</v>
       </c>
       <c r="N32">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>-169827.98000000045</v>
       </c>
       <c r="O32" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>-2.7581118653977402E-2</v>
       </c>
       <c r="P32">
-        <f t="shared" si="8"/>
+        <f>RANK(O32,$O:$O,1)</f>
         <v>23</v>
       </c>
     </row>
@@ -3095,7 +3112,7 @@
         <v>-7.9969930789269058E-3</v>
       </c>
       <c r="F33">
-        <f t="shared" si="2"/>
+        <f>_xlfn.RANK.EQ(E33,$E:$E,1)</f>
         <v>41</v>
       </c>
       <c r="G33">
@@ -3105,15 +3122,15 @@
         <v>977068513.48000002</v>
       </c>
       <c r="I33">
+        <f t="shared" si="2"/>
+        <v>-2602486.5199999809</v>
+      </c>
+      <c r="J33" s="5">
         <f t="shared" si="3"/>
-        <v>-2602486.5199999809</v>
-      </c>
-      <c r="J33" s="5">
-        <f t="shared" si="4"/>
         <v>-2.6564903115433454E-3</v>
       </c>
       <c r="K33">
-        <f t="shared" si="5"/>
+        <f>RANK(J33,$J:$J,1)</f>
         <v>43</v>
       </c>
       <c r="L33">
@@ -3123,15 +3140,15 @@
         <v>984116289.40999901</v>
       </c>
       <c r="N33">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>-5456610.5900000334</v>
       </c>
       <c r="O33" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>-5.5141067323084929E-3</v>
       </c>
       <c r="P33">
-        <f t="shared" si="8"/>
+        <f>RANK(O33,$O:$O,1)</f>
         <v>34</v>
       </c>
     </row>
@@ -3154,7 +3171,7 @@
         <v>-1.8939149738619768E-2</v>
       </c>
       <c r="F34">
-        <f t="shared" si="2"/>
+        <f>_xlfn.RANK.EQ(E34,$E:$E,1)</f>
         <v>26</v>
       </c>
       <c r="G34">
@@ -3164,15 +3181,15 @@
         <v>4137588.7699999898</v>
       </c>
       <c r="I34">
+        <f t="shared" si="2"/>
+        <v>-213011.23000001023</v>
+      </c>
+      <c r="J34" s="5">
         <f t="shared" si="3"/>
-        <v>-213011.23000001023</v>
-      </c>
-      <c r="J34" s="5">
-        <f t="shared" si="4"/>
         <v>-4.8961345561534093E-2</v>
       </c>
       <c r="K34">
-        <f t="shared" si="5"/>
+        <f>RANK(J34,$J:$J,1)</f>
         <v>21</v>
       </c>
       <c r="L34">
@@ -3182,15 +3199,15 @@
         <v>4229801.51</v>
       </c>
       <c r="N34">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>-115798.49000000022</v>
       </c>
       <c r="O34" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>-2.6647296115611244E-2</v>
       </c>
       <c r="P34">
-        <f t="shared" si="8"/>
+        <f>RANK(O34,$O:$O,1)</f>
         <v>24</v>
       </c>
     </row>
@@ -3213,43 +3230,43 @@
         <v>0</v>
       </c>
       <c r="F35">
+        <f>_xlfn.RANK.EQ(E35,$E:$E,1)</f>
+        <v>47</v>
+      </c>
+      <c r="G35">
+        <v>0</v>
+      </c>
+      <c r="H35">
+        <v>0</v>
+      </c>
+      <c r="I35">
         <f t="shared" si="2"/>
-        <v>47</v>
-      </c>
-      <c r="G35">
-        <v>0</v>
-      </c>
-      <c r="H35">
-        <v>0</v>
-      </c>
-      <c r="I35">
+        <v>0</v>
+      </c>
+      <c r="J35" s="5">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J35" s="5">
+      <c r="K35">
+        <f>RANK(J35,$J:$J,1)</f>
+        <v>48</v>
+      </c>
+      <c r="L35">
+        <v>0</v>
+      </c>
+      <c r="M35">
+        <v>0</v>
+      </c>
+      <c r="N35">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="K35">
+      <c r="O35" s="5">
         <f t="shared" si="5"/>
-        <v>48</v>
-      </c>
-      <c r="L35">
-        <v>0</v>
-      </c>
-      <c r="M35">
-        <v>0</v>
-      </c>
-      <c r="N35">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="O35" s="5">
-        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="P35">
-        <f t="shared" si="8"/>
+        <f>RANK(O35,$O:$O,1)</f>
         <v>48</v>
       </c>
     </row>
@@ -3272,7 +3289,7 @@
         <v>-7.8647857679780775E-2</v>
       </c>
       <c r="F36">
-        <f t="shared" si="2"/>
+        <f>_xlfn.RANK.EQ(E36,$E:$E,1)</f>
         <v>10</v>
       </c>
       <c r="G36">
@@ -3282,15 +3299,15 @@
         <v>740966.94999999902</v>
       </c>
       <c r="I36">
+        <f t="shared" si="2"/>
+        <v>-157733.05000000098</v>
+      </c>
+      <c r="J36" s="5">
         <f t="shared" si="3"/>
-        <v>-157733.05000000098</v>
-      </c>
-      <c r="J36" s="5">
-        <f t="shared" si="4"/>
         <v>-0.17551246244575608</v>
       </c>
       <c r="K36">
-        <f t="shared" si="5"/>
+        <f>RANK(J36,$J:$J,1)</f>
         <v>1</v>
       </c>
       <c r="L36">
@@ -3300,15 +3317,15 @@
         <v>777215.28999999899</v>
       </c>
       <c r="N36">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>-101084.71000000101</v>
       </c>
       <c r="O36" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>-0.11509132414892521</v>
       </c>
       <c r="P36">
-        <f t="shared" si="8"/>
+        <f>RANK(O36,$O:$O,1)</f>
         <v>5</v>
       </c>
     </row>
@@ -3331,7 +3348,7 @@
         <v>-3.9444515758219188E-2</v>
       </c>
       <c r="F37">
-        <f t="shared" si="2"/>
+        <f>_xlfn.RANK.EQ(E37,$E:$E,1)</f>
         <v>19</v>
       </c>
       <c r="G37">
@@ -3341,15 +3358,15 @@
         <v>2118943.21</v>
       </c>
       <c r="I37">
+        <f t="shared" si="2"/>
+        <v>-110256.79000000004</v>
+      </c>
+      <c r="J37" s="5">
         <f t="shared" si="3"/>
-        <v>-110256.79000000004</v>
-      </c>
-      <c r="J37" s="5">
-        <f t="shared" si="4"/>
         <v>-4.9460250314014013E-2</v>
       </c>
       <c r="K37">
-        <f t="shared" si="5"/>
+        <f>RANK(J37,$J:$J,1)</f>
         <v>20</v>
       </c>
       <c r="L37">
@@ -3359,15 +3376,15 @@
         <v>2108718.34</v>
       </c>
       <c r="N37">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>-188181.66000000015</v>
       </c>
       <c r="O37" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>-8.1928538464887526E-2</v>
       </c>
       <c r="P37">
-        <f t="shared" si="8"/>
+        <f>RANK(O37,$O:$O,1)</f>
         <v>8</v>
       </c>
     </row>
@@ -3390,7 +3407,7 @@
         <v>-1.9443680579913542E-2</v>
       </c>
       <c r="F38">
-        <f t="shared" si="2"/>
+        <f>_xlfn.RANK.EQ(E38,$E:$E,1)</f>
         <v>25</v>
       </c>
       <c r="G38">
@@ -3400,15 +3417,15 @@
         <v>753451.96</v>
       </c>
       <c r="I38">
+        <f t="shared" si="2"/>
+        <v>-39348.040000000037</v>
+      </c>
+      <c r="J38" s="5">
         <f t="shared" si="3"/>
-        <v>-39348.040000000037</v>
-      </c>
-      <c r="J38" s="5">
-        <f t="shared" si="4"/>
         <v>-4.9631735620585316E-2</v>
       </c>
       <c r="K38">
-        <f t="shared" si="5"/>
+        <f>RANK(J38,$J:$J,1)</f>
         <v>19</v>
       </c>
       <c r="L38">
@@ -3418,15 +3435,15 @@
         <v>777663.26</v>
       </c>
       <c r="N38">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>-136.73999999999069</v>
       </c>
       <c r="O38" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>-1.7580354847003174E-4</v>
       </c>
       <c r="P38">
-        <f t="shared" si="8"/>
+        <f>RANK(O38,$O:$O,1)</f>
         <v>40</v>
       </c>
     </row>
@@ -3449,7 +3466,7 @@
         <v>-8.008952370177623E-2</v>
       </c>
       <c r="F39">
-        <f t="shared" si="2"/>
+        <f>_xlfn.RANK.EQ(E39,$E:$E,1)</f>
         <v>8</v>
       </c>
       <c r="G39">
@@ -3459,15 +3476,15 @@
         <v>1114242.27999999</v>
       </c>
       <c r="I39">
+        <f t="shared" si="2"/>
+        <v>-180157.72000000998</v>
+      </c>
+      <c r="J39" s="5">
         <f t="shared" si="3"/>
-        <v>-180157.72000000998</v>
-      </c>
-      <c r="J39" s="5">
-        <f t="shared" si="4"/>
         <v>-0.13918241656366656</v>
       </c>
       <c r="K39">
-        <f t="shared" si="5"/>
+        <f>RANK(J39,$J:$J,1)</f>
         <v>3</v>
       </c>
       <c r="L39">
@@ -3477,15 +3494,15 @@
         <v>1680463.8699999901</v>
       </c>
       <c r="N39">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>-79036.1300000099</v>
       </c>
       <c r="O39" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>-4.4919653310605226E-2</v>
       </c>
       <c r="P39">
-        <f t="shared" si="8"/>
+        <f>RANK(O39,$O:$O,1)</f>
         <v>17</v>
       </c>
     </row>
@@ -3508,7 +3525,7 @@
         <v>-2.1279773539092578E-2</v>
       </c>
       <c r="F40">
-        <f t="shared" si="2"/>
+        <f>_xlfn.RANK.EQ(E40,$E:$E,1)</f>
         <v>23</v>
       </c>
       <c r="G40">
@@ -3518,15 +3535,15 @@
         <v>38095240.189999901</v>
       </c>
       <c r="I40">
+        <f t="shared" si="2"/>
+        <v>-1869659.8100000992</v>
+      </c>
+      <c r="J40" s="5">
         <f t="shared" si="3"/>
-        <v>-1869659.8100000992</v>
-      </c>
-      <c r="J40" s="5">
-        <f t="shared" si="4"/>
         <v>-4.6782546934937892E-2</v>
       </c>
       <c r="K40">
-        <f t="shared" si="5"/>
+        <f>RANK(J40,$J:$J,1)</f>
         <v>22</v>
       </c>
       <c r="L40">
@@ -3536,15 +3553,15 @@
         <v>39606263.709999897</v>
       </c>
       <c r="N40">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>-610436.29000010341</v>
       </c>
       <c r="O40" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>-1.5178676768608648E-2</v>
       </c>
       <c r="P40">
-        <f t="shared" si="8"/>
+        <f>RANK(O40,$O:$O,1)</f>
         <v>31</v>
       </c>
     </row>
@@ -3567,7 +3584,7 @@
         <v>-4.0110550149132493E-2</v>
       </c>
       <c r="F41">
-        <f t="shared" si="2"/>
+        <f>_xlfn.RANK.EQ(E41,$E:$E,1)</f>
         <v>17</v>
       </c>
       <c r="G41">
@@ -3577,15 +3594,15 @@
         <v>4956043.6699999897</v>
       </c>
       <c r="I41">
+        <f t="shared" si="2"/>
+        <v>-133456.33000001032</v>
+      </c>
+      <c r="J41" s="5">
         <f t="shared" si="3"/>
-        <v>-133456.33000001032</v>
-      </c>
-      <c r="J41" s="5">
-        <f t="shared" si="4"/>
         <v>-2.6221894095689226E-2</v>
       </c>
       <c r="K41">
-        <f t="shared" si="5"/>
+        <f>RANK(J41,$J:$J,1)</f>
         <v>34</v>
       </c>
       <c r="L41">
@@ -3595,15 +3612,15 @@
         <v>4717822.6500000004</v>
       </c>
       <c r="N41">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>-82077.349999999627</v>
       </c>
       <c r="O41" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>-1.7099804162586642E-2</v>
       </c>
       <c r="P41">
-        <f t="shared" si="8"/>
+        <f>RANK(O41,$O:$O,1)</f>
         <v>30</v>
       </c>
     </row>
@@ -3626,7 +3643,7 @@
         <v>-2.2070943135841053E-4</v>
       </c>
       <c r="F42">
-        <f t="shared" si="2"/>
+        <f>_xlfn.RANK.EQ(E42,$E:$E,1)</f>
         <v>44</v>
       </c>
       <c r="G42">
@@ -3636,15 +3653,15 @@
         <v>196755033.31</v>
       </c>
       <c r="I42">
+        <f t="shared" si="2"/>
+        <v>-2375266.6899999976</v>
+      </c>
+      <c r="J42" s="5">
         <f t="shared" si="3"/>
-        <v>-2375266.6899999976</v>
-      </c>
-      <c r="J42" s="5">
-        <f t="shared" si="4"/>
         <v>-1.1928203241796942E-2</v>
       </c>
       <c r="K42">
-        <f t="shared" si="5"/>
+        <f>RANK(J42,$J:$J,1)</f>
         <v>39</v>
       </c>
       <c r="L42">
@@ -3654,15 +3671,15 @@
         <v>199954563.74999899</v>
       </c>
       <c r="N42">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>-36.250001013278961</v>
       </c>
       <c r="O42" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>-1.8129115815929696E-7</v>
       </c>
       <c r="P42">
-        <f t="shared" si="8"/>
+        <f>RANK(O42,$O:$O,1)</f>
         <v>47</v>
       </c>
     </row>
@@ -3685,7 +3702,7 @@
         <v>-2.0497353541313264E-2</v>
       </c>
       <c r="F43">
-        <f t="shared" si="2"/>
+        <f>_xlfn.RANK.EQ(E43,$E:$E,1)</f>
         <v>24</v>
       </c>
       <c r="G43">
@@ -3695,15 +3712,15 @@
         <v>8171472.0199999996</v>
       </c>
       <c r="I43">
+        <f t="shared" si="2"/>
+        <v>-389327.98000000045</v>
+      </c>
+      <c r="J43" s="5">
         <f t="shared" si="3"/>
-        <v>-389327.98000000045</v>
-      </c>
-      <c r="J43" s="5">
-        <f t="shared" si="4"/>
         <v>-4.5477990374731388E-2</v>
       </c>
       <c r="K43">
-        <f t="shared" si="5"/>
+        <f>RANK(J43,$J:$J,1)</f>
         <v>23</v>
       </c>
       <c r="L43">
@@ -3713,15 +3730,15 @@
         <v>8150982.5699999901</v>
       </c>
       <c r="N43">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>-346517.43000000995</v>
       </c>
       <c r="O43" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>-4.0778750220654303E-2</v>
       </c>
       <c r="P43">
-        <f t="shared" si="8"/>
+        <f>RANK(O43,$O:$O,1)</f>
         <v>18</v>
       </c>
     </row>
@@ -3744,7 +3761,7 @@
         <v>-9.7760750186150751E-3</v>
       </c>
       <c r="F44">
-        <f t="shared" si="2"/>
+        <f>_xlfn.RANK.EQ(E44,$E:$E,1)</f>
         <v>39</v>
       </c>
       <c r="G44">
@@ -3754,15 +3771,15 @@
         <v>30793711.48</v>
       </c>
       <c r="I44">
+        <f t="shared" si="2"/>
+        <v>-246988.51999999955</v>
+      </c>
+      <c r="J44" s="5">
         <f t="shared" si="3"/>
-        <v>-246988.51999999955</v>
-      </c>
-      <c r="J44" s="5">
-        <f t="shared" si="4"/>
         <v>-7.9569249404813532E-3</v>
       </c>
       <c r="K44">
-        <f t="shared" si="5"/>
+        <f>RANK(J44,$J:$J,1)</f>
         <v>41</v>
       </c>
       <c r="L44">
@@ -3772,15 +3789,15 @@
         <v>31282141.25</v>
       </c>
       <c r="N44">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>-58.75</v>
       </c>
       <c r="O44" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>-1.8780648419868168E-6</v>
       </c>
       <c r="P44">
-        <f t="shared" si="8"/>
+        <f>RANK(O44,$O:$O,1)</f>
         <v>45</v>
       </c>
     </row>
@@ -3803,7 +3820,7 @@
         <v>-1.287514194887851E-2</v>
       </c>
       <c r="F45">
-        <f t="shared" si="2"/>
+        <f>_xlfn.RANK.EQ(E45,$E:$E,1)</f>
         <v>34</v>
       </c>
       <c r="G45">
@@ -3813,15 +3830,15 @@
         <v>54594953.959999897</v>
       </c>
       <c r="I45">
+        <f t="shared" si="2"/>
+        <v>-2197246.0400001034</v>
+      </c>
+      <c r="J45" s="5">
         <f t="shared" si="3"/>
-        <v>-2197246.0400001034</v>
-      </c>
-      <c r="J45" s="5">
-        <f t="shared" si="4"/>
         <v>-3.8689222111488959E-2</v>
       </c>
       <c r="K45">
-        <f t="shared" si="5"/>
+        <f>RANK(J45,$J:$J,1)</f>
         <v>30</v>
       </c>
       <c r="L45">
@@ -3831,15 +3848,15 @@
         <v>55386549.6599999</v>
       </c>
       <c r="N45">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>-640550.34000010043</v>
       </c>
       <c r="O45" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>-1.1432866237947358E-2</v>
       </c>
       <c r="P45">
-        <f t="shared" si="8"/>
+        <f>RANK(O45,$O:$O,1)</f>
         <v>32</v>
       </c>
     </row>
@@ -3862,7 +3879,7 @@
         <v>-3.0010420686993711E-3</v>
       </c>
       <c r="F46">
-        <f t="shared" si="2"/>
+        <f>_xlfn.RANK.EQ(E46,$E:$E,1)</f>
         <v>43</v>
       </c>
       <c r="G46">
@@ -3872,15 +3889,15 @@
         <v>257402.90999999901</v>
       </c>
       <c r="I46">
+        <f t="shared" si="2"/>
+        <v>-8597.090000000986</v>
+      </c>
+      <c r="J46" s="5">
         <f t="shared" si="3"/>
-        <v>-8597.090000000986</v>
-      </c>
-      <c r="J46" s="5">
-        <f t="shared" si="4"/>
         <v>-3.2319887218048821E-2</v>
       </c>
       <c r="K46">
-        <f t="shared" si="5"/>
+        <f>RANK(J46,$J:$J,1)</f>
         <v>33</v>
       </c>
       <c r="L46">
@@ -3890,15 +3907,15 @@
         <v>254753.15999999901</v>
       </c>
       <c r="N46">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>-12346.840000000986</v>
       </c>
       <c r="O46" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>-4.6225533508053113E-2</v>
       </c>
       <c r="P46">
-        <f t="shared" si="8"/>
+        <f>RANK(O46,$O:$O,1)</f>
         <v>16</v>
       </c>
     </row>
@@ -3921,7 +3938,7 @@
         <v>-1.7435939690898361E-4</v>
       </c>
       <c r="F47">
-        <f t="shared" si="2"/>
+        <f>_xlfn.RANK.EQ(E47,$E:$E,1)</f>
         <v>45</v>
       </c>
       <c r="G47">
@@ -3931,15 +3948,15 @@
         <v>73442541.659999996</v>
       </c>
       <c r="I47">
+        <f t="shared" si="2"/>
+        <v>-24458.340000003576</v>
+      </c>
+      <c r="J47" s="5">
         <f t="shared" si="3"/>
-        <v>-24458.340000003576</v>
-      </c>
-      <c r="J47" s="5">
-        <f t="shared" si="4"/>
         <v>-3.3291600310348285E-4</v>
       </c>
       <c r="K47">
-        <f t="shared" si="5"/>
+        <f>RANK(J47,$J:$J,1)</f>
         <v>45</v>
       </c>
       <c r="L47">
@@ -3949,15 +3966,15 @@
         <v>75050829.179999903</v>
       </c>
       <c r="N47">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>-21970.820000097156</v>
       </c>
       <c r="O47" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>-2.9266019117572752E-4</v>
       </c>
       <c r="P47">
-        <f t="shared" si="8"/>
+        <f>RANK(O47,$O:$O,1)</f>
         <v>38</v>
       </c>
     </row>
@@ -3980,7 +3997,7 @@
         <v>-3.1133192323107857E-2</v>
       </c>
       <c r="F48">
-        <f t="shared" si="2"/>
+        <f>_xlfn.RANK.EQ(E48,$E:$E,1)</f>
         <v>20</v>
       </c>
       <c r="G48">
@@ -3990,15 +4007,15 @@
         <v>6922072.5599999996</v>
       </c>
       <c r="I48">
+        <f t="shared" si="2"/>
+        <v>-292627.44000000041</v>
+      </c>
+      <c r="J48" s="5">
         <f t="shared" si="3"/>
-        <v>-292627.44000000041</v>
-      </c>
-      <c r="J48" s="5">
-        <f t="shared" si="4"/>
         <v>-4.0559890224125802E-2</v>
       </c>
       <c r="K48">
-        <f t="shared" si="5"/>
+        <f>RANK(J48,$J:$J,1)</f>
         <v>29</v>
       </c>
       <c r="L48">
@@ -4008,15 +4025,15 @@
         <v>6882350.23999999</v>
       </c>
       <c r="N48">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>-407449.76000001002</v>
       </c>
       <c r="O48" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>-5.5893132870587676E-2</v>
       </c>
       <c r="P48">
-        <f t="shared" si="8"/>
+        <f>RANK(O48,$O:$O,1)</f>
         <v>15</v>
       </c>
     </row>
@@ -4039,7 +4056,7 @@
         <v>-1.8444360086767971E-2</v>
       </c>
       <c r="F49">
-        <f t="shared" si="2"/>
+        <f>_xlfn.RANK.EQ(E49,$E:$E,1)</f>
         <v>27</v>
       </c>
       <c r="G49">
@@ -4049,33 +4066,33 @@
         <v>95466.880000000005</v>
       </c>
       <c r="I49">
+        <f t="shared" si="2"/>
+        <v>-7133.1199999999953</v>
+      </c>
+      <c r="J49" s="5">
         <f t="shared" si="3"/>
-        <v>-7133.1199999999953</v>
-      </c>
-      <c r="J49" s="5">
+        <v>-6.9523586744639335E-2</v>
+      </c>
+      <c r="K49">
+        <f>RANK(J49,$J:$J,1)</f>
+        <v>13</v>
+      </c>
+      <c r="L49">
+        <v>0</v>
+      </c>
+      <c r="M49">
+        <v>0</v>
+      </c>
+      <c r="N49">
         <f t="shared" si="4"/>
-        <v>-6.9523586744639335E-2</v>
-      </c>
-      <c r="K49">
+        <v>0</v>
+      </c>
+      <c r="O49" s="5">
         <f t="shared" si="5"/>
-        <v>13</v>
-      </c>
-      <c r="L49">
-        <v>0</v>
-      </c>
-      <c r="M49">
-        <v>0</v>
-      </c>
-      <c r="N49">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="O49" s="5">
-        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="P49">
-        <f t="shared" si="8"/>
+        <f>RANK(O49,$O:$O,1)</f>
         <v>48</v>
       </c>
     </row>
@@ -4098,7 +4115,7 @@
         <v>0</v>
       </c>
       <c r="F50">
-        <f t="shared" si="2"/>
+        <f>_xlfn.RANK.EQ(E50,$E:$E,1)</f>
         <v>47</v>
       </c>
       <c r="G50">
@@ -4108,15 +4125,15 @@
         <v>859100</v>
       </c>
       <c r="I50">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J50" s="5">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J50" s="5">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
       <c r="K50">
-        <f t="shared" si="5"/>
+        <f>RANK(J50,$J:$J,1)</f>
         <v>48</v>
       </c>
       <c r="L50">
@@ -4126,15 +4143,15 @@
         <v>843200</v>
       </c>
       <c r="N50">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="O50" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="P50">
-        <f t="shared" si="8"/>
+        <f>RANK(O50,$O:$O,1)</f>
         <v>48</v>
       </c>
     </row>
@@ -4157,7 +4174,7 @@
         <v>-1.2785255822058129E-2</v>
       </c>
       <c r="F51">
-        <f t="shared" si="2"/>
+        <f>_xlfn.RANK.EQ(E51,$E:$E,1)</f>
         <v>35</v>
       </c>
       <c r="G51">
@@ -4167,15 +4184,15 @@
         <v>8599059.6199999992</v>
       </c>
       <c r="I51">
+        <f t="shared" si="2"/>
+        <v>-326440.38000000082</v>
+      </c>
+      <c r="J51" s="5">
         <f t="shared" si="3"/>
-        <v>-326440.38000000082</v>
-      </c>
-      <c r="J51" s="5">
-        <f t="shared" si="4"/>
         <v>-3.6573903982970231E-2</v>
       </c>
       <c r="K51">
-        <f t="shared" si="5"/>
+        <f>RANK(J51,$J:$J,1)</f>
         <v>31</v>
       </c>
       <c r="L51">
@@ -4185,15 +4202,15 @@
         <v>8735843.3100000005</v>
       </c>
       <c r="N51">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>-98056.689999999478</v>
       </c>
       <c r="O51" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>-1.1100045280114048E-2</v>
       </c>
       <c r="P51">
-        <f t="shared" si="8"/>
+        <f>RANK(O51,$O:$O,1)</f>
         <v>33</v>
       </c>
     </row>
@@ -4216,7 +4233,7 @@
         <v>-8.009596083231342E-2</v>
       </c>
       <c r="F52">
-        <f t="shared" si="2"/>
+        <f>_xlfn.RANK.EQ(E52,$E:$E,1)</f>
         <v>7</v>
       </c>
       <c r="G52">
@@ -4226,15 +4243,15 @@
         <v>2204672.88</v>
       </c>
       <c r="I52">
+        <f t="shared" si="2"/>
+        <v>-236027.12000000011</v>
+      </c>
+      <c r="J52" s="5">
         <f t="shared" si="3"/>
-        <v>-236027.12000000011</v>
-      </c>
-      <c r="J52" s="5">
-        <f t="shared" si="4"/>
         <v>-9.6704683082722218E-2</v>
       </c>
       <c r="K52">
-        <f t="shared" si="5"/>
+        <f>RANK(J52,$J:$J,1)</f>
         <v>9</v>
       </c>
       <c r="L52">
@@ -4244,15 +4261,15 @@
         <v>2056835.26</v>
       </c>
       <c r="N52">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>-264764.74</v>
       </c>
       <c r="O52" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>-0.11404408166781529</v>
       </c>
       <c r="P52">
-        <f t="shared" si="8"/>
+        <f>RANK(O52,$O:$O,1)</f>
         <v>6</v>
       </c>
     </row>
@@ -4297,15 +4314,15 @@
         <v>25</v>
       </c>
       <c r="B57">
-        <f t="shared" ref="B57:B61" si="9">VLOOKUP(A57,$A$2:$E$52,4,FALSE)</f>
+        <f t="shared" ref="B57:B61" si="6">VLOOKUP(A57,$A$2:$E$52,4,FALSE)</f>
         <v>0</v>
       </c>
       <c r="C57">
-        <f t="shared" ref="C57:D61" si="10">VLOOKUP(A57,$A$2:$P$52,9,FALSE)</f>
+        <f t="shared" ref="C57:C61" si="7">VLOOKUP(A57,$A$2:$P$52,9,FALSE)</f>
         <v>0</v>
       </c>
       <c r="D57">
-        <f t="shared" ref="D57:D61" si="11">VLOOKUP(A57,$A$2:$P$52,14,FALSE)</f>
+        <f t="shared" ref="D57:D61" si="8">VLOOKUP(A57,$A$2:$P$52,14,FALSE)</f>
         <v>-311228.08999999997</v>
       </c>
     </row>
@@ -4314,15 +4331,15 @@
         <v>32</v>
       </c>
       <c r="B58">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>-149396.10000000987</v>
       </c>
       <c r="C58">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v>-189254.06000000006</v>
       </c>
       <c r="D58">
-        <f t="shared" si="11"/>
+        <f t="shared" si="8"/>
         <v>-374962.91000000015</v>
       </c>
     </row>
@@ -4331,15 +4348,15 @@
         <v>38</v>
       </c>
       <c r="B59">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>-12230.810000000056</v>
       </c>
       <c r="C59">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v>-45485.580000000075</v>
       </c>
       <c r="D59">
-        <f t="shared" si="11"/>
+        <f t="shared" si="8"/>
         <v>-72.879999999888241</v>
       </c>
     </row>
@@ -4348,15 +4365,15 @@
         <v>39</v>
       </c>
       <c r="B60">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>-4950.4699999999721</v>
       </c>
       <c r="C60">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v>-8005.7900000010268</v>
       </c>
       <c r="D60">
-        <f t="shared" si="11"/>
+        <f t="shared" si="8"/>
         <v>-1724.9000000000233</v>
       </c>
     </row>
@@ -4365,21 +4382,21 @@
         <v>55</v>
       </c>
       <c r="B61">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>-184239.79000001028</v>
       </c>
       <c r="C61">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v>-133456.33000001032</v>
       </c>
       <c r="D61">
-        <f t="shared" si="11"/>
+        <f t="shared" si="8"/>
         <v>-82077.349999999627</v>
       </c>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A63" s="7" t="s">
-        <v>68</v>
+      <c r="A63" s="10" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.35">
@@ -4401,15 +4418,15 @@
         <v>24</v>
       </c>
       <c r="B65">
-        <f>_xlfn.XLOOKUP(A65,A2:A52,D2:D52,,0)</f>
+        <f>VLOOKUP($A65,$A$1:$P$52,MATCH(B$64,$1:$1,0),FALSE)</f>
         <v>-36209.630000000005</v>
       </c>
       <c r="C65">
-        <f>_xlfn.XLOOKUP(A65,$A$2:$A$52,$I$2:$I$52,,0)</f>
+        <f t="shared" ref="C65:D65" si="9">VLOOKUP($A65,$A$1:$P$52,MATCH(C$64,$1:$1,0),FALSE)</f>
         <v>-27292.159999999974</v>
       </c>
       <c r="D65">
-        <f>_xlfn.XLOOKUP(A65,$A$2:$A$52,$N$2:$N$52,,0)</f>
+        <f t="shared" si="9"/>
         <v>-9181.0800000000163</v>
       </c>
     </row>
@@ -4418,15 +4435,15 @@
         <v>25</v>
       </c>
       <c r="B66">
-        <f t="shared" ref="B66:B70" si="12">_xlfn.XLOOKUP(A66,A3:A53,D3:D53,,0)</f>
+        <f t="shared" ref="B66:D70" si="10">VLOOKUP($A66,$A$1:$P$52,MATCH(B$64,$1:$1,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="C66">
-        <f t="shared" ref="C66:C70" si="13">_xlfn.XLOOKUP(A66,$A$2:$A$52,$I$2:$I$52,,0)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="D66">
-        <f t="shared" ref="D66:D70" si="14">_xlfn.XLOOKUP(A66,$A$2:$A$52,$N$2:$N$52,,0)</f>
+        <f t="shared" si="10"/>
         <v>-311228.08999999997</v>
       </c>
     </row>
@@ -4435,15 +4452,15 @@
         <v>32</v>
       </c>
       <c r="B67">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>-149396.10000000987</v>
       </c>
       <c r="C67">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v>-189254.06000000006</v>
       </c>
       <c r="D67">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>-374962.91000000015</v>
       </c>
     </row>
@@ -4452,15 +4469,15 @@
         <v>38</v>
       </c>
       <c r="B68">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>-12230.810000000056</v>
       </c>
       <c r="C68">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v>-45485.580000000075</v>
       </c>
       <c r="D68">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>-72.879999999888241</v>
       </c>
     </row>
@@ -4469,15 +4486,15 @@
         <v>39</v>
       </c>
       <c r="B69">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>-4950.4699999999721</v>
       </c>
       <c r="C69">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v>-8005.7900000010268</v>
       </c>
       <c r="D69">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>-1724.9000000000233</v>
       </c>
     </row>
@@ -4486,21 +4503,21 @@
         <v>55</v>
       </c>
       <c r="B70">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>-184239.79000001028</v>
       </c>
       <c r="C70">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v>-133456.33000001032</v>
       </c>
       <c r="D70">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>-82077.349999999627</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A72" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.35">
@@ -4522,15 +4539,15 @@
         <v>24</v>
       </c>
       <c r="B74">
-        <f>INDEX($D$2:$D$52,MATCH(A74,$A$2:$A$52,0))</f>
+        <f>_xlfn.XLOOKUP(A74,$A$2:$A$52,$D$2:$D$52,,0)</f>
         <v>-36209.630000000005</v>
       </c>
       <c r="C74">
-        <f>INDEX($I$2:$I$52,MATCH(A74,$A$2:$A$52,0))</f>
+        <f>_xlfn.XLOOKUP(A74,$A$2:$A$52,$I$2:$I$52,,0)</f>
         <v>-27292.159999999974</v>
       </c>
       <c r="D74">
-        <f>INDEX($N$2:$N$52,MATCH(A74,$A$2:$A$52,0))</f>
+        <f>_xlfn.XLOOKUP(A74,$A$2:$A$52,$N$2:$N$52,,0)</f>
         <v>-9181.0800000000163</v>
       </c>
     </row>
@@ -4539,15 +4556,15 @@
         <v>25</v>
       </c>
       <c r="B75">
-        <f t="shared" ref="B75:B79" si="15">INDEX($D$2:$D$52,MATCH(A75,$A$2:$A$52,0))</f>
+        <f t="shared" ref="B75:B79" si="11">_xlfn.XLOOKUP(A75,$A$2:$A$52,$D$2:$D$52,,0)</f>
         <v>0</v>
       </c>
       <c r="C75">
-        <f t="shared" ref="C75:C79" si="16">INDEX($I$2:$I$52,MATCH(A75,$A$2:$A$52,0))</f>
+        <f t="shared" ref="C75:C79" si="12">_xlfn.XLOOKUP(A75,$A$2:$A$52,$I$2:$I$52,,0)</f>
         <v>0</v>
       </c>
       <c r="D75">
-        <f t="shared" ref="D75:D79" si="17">INDEX($N$2:$N$52,MATCH(A75,$A$2:$A$52,0))</f>
+        <f t="shared" ref="D75:D79" si="13">_xlfn.XLOOKUP(A75,$A$2:$A$52,$N$2:$N$52,,0)</f>
         <v>-311228.08999999997</v>
       </c>
     </row>
@@ -4556,15 +4573,15 @@
         <v>32</v>
       </c>
       <c r="B76">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>-149396.10000000987</v>
       </c>
       <c r="C76">
-        <f t="shared" si="16"/>
+        <f t="shared" si="12"/>
         <v>-189254.06000000006</v>
       </c>
       <c r="D76">
-        <f t="shared" si="17"/>
+        <f t="shared" si="13"/>
         <v>-374962.91000000015</v>
       </c>
     </row>
@@ -4573,15 +4590,15 @@
         <v>38</v>
       </c>
       <c r="B77">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>-12230.810000000056</v>
       </c>
       <c r="C77">
-        <f t="shared" si="16"/>
+        <f t="shared" si="12"/>
         <v>-45485.580000000075</v>
       </c>
       <c r="D77">
-        <f t="shared" si="17"/>
+        <f t="shared" si="13"/>
         <v>-72.879999999888241</v>
       </c>
     </row>
@@ -4590,15 +4607,15 @@
         <v>39</v>
       </c>
       <c r="B78">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>-4950.4699999999721</v>
       </c>
       <c r="C78">
-        <f t="shared" si="16"/>
+        <f t="shared" si="12"/>
         <v>-8005.7900000010268</v>
       </c>
       <c r="D78">
-        <f t="shared" si="17"/>
+        <f t="shared" si="13"/>
         <v>-1724.9000000000233</v>
       </c>
     </row>
@@ -4607,222 +4624,446 @@
         <v>55</v>
       </c>
       <c r="B79">
+        <f t="shared" si="11"/>
+        <v>-184239.79000001028</v>
+      </c>
+      <c r="C79">
+        <f t="shared" si="12"/>
+        <v>-133456.33000001032</v>
+      </c>
+      <c r="D79">
+        <f t="shared" si="13"/>
+        <v>-82077.349999999627</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A81" s="7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A82" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A83" t="s">
+        <v>24</v>
+      </c>
+      <c r="B83" t="e">
+        <f>_xlfn.XLOOKUP(A83,A2:P52,MATCH(B82,1:1,0),,0)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E83">
+        <f>MATCH(B82,1:1,0)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A84" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A85" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A86" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A87" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A88" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A90" s="7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A91" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A92" t="s">
+        <v>24</v>
+      </c>
+      <c r="B92">
+        <f>INDEX($D$2:$D$52,MATCH(A92,$A$2:$A$52,0))</f>
+        <v>-36209.630000000005</v>
+      </c>
+      <c r="C92">
+        <f>INDEX($I$2:$I$52,MATCH(A92,$A$2:$A$52,0))</f>
+        <v>-27292.159999999974</v>
+      </c>
+      <c r="D92">
+        <f>INDEX($N$2:$N$52,MATCH(A92,$A$2:$A$52,0))</f>
+        <v>-9181.0800000000163</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A93" t="s">
+        <v>25</v>
+      </c>
+      <c r="B93">
+        <f t="shared" ref="B93:B97" si="14">INDEX($D$2:$D$52,MATCH(A93,$A$2:$A$52,0))</f>
+        <v>0</v>
+      </c>
+      <c r="C93">
+        <f t="shared" ref="C93:C97" si="15">INDEX($I$2:$I$52,MATCH(A93,$A$2:$A$52,0))</f>
+        <v>0</v>
+      </c>
+      <c r="D93">
+        <f t="shared" ref="D93:D97" si="16">INDEX($N$2:$N$52,MATCH(A93,$A$2:$A$52,0))</f>
+        <v>-311228.08999999997</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A94" t="s">
+        <v>32</v>
+      </c>
+      <c r="B94">
+        <f t="shared" si="14"/>
+        <v>-149396.10000000987</v>
+      </c>
+      <c r="C94">
         <f t="shared" si="15"/>
+        <v>-189254.06000000006</v>
+      </c>
+      <c r="D94">
+        <f t="shared" si="16"/>
+        <v>-374962.91000000015</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A95" t="s">
+        <v>38</v>
+      </c>
+      <c r="B95">
+        <f t="shared" si="14"/>
+        <v>-12230.810000000056</v>
+      </c>
+      <c r="C95">
+        <f t="shared" si="15"/>
+        <v>-45485.580000000075</v>
+      </c>
+      <c r="D95">
+        <f t="shared" si="16"/>
+        <v>-72.879999999888241</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A96" t="s">
+        <v>39</v>
+      </c>
+      <c r="B96">
+        <f t="shared" si="14"/>
+        <v>-4950.4699999999721</v>
+      </c>
+      <c r="C96">
+        <f t="shared" si="15"/>
+        <v>-8005.7900000010268</v>
+      </c>
+      <c r="D96">
+        <f t="shared" si="16"/>
+        <v>-1724.9000000000233</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A97" t="s">
+        <v>55</v>
+      </c>
+      <c r="B97">
+        <f t="shared" si="14"/>
         <v>-184239.79000001028</v>
       </c>
-      <c r="C79">
+      <c r="C97">
+        <f t="shared" si="15"/>
+        <v>-133456.33000001032</v>
+      </c>
+      <c r="D97">
         <f t="shared" si="16"/>
-        <v>-133456.33000001032</v>
-      </c>
-      <c r="D79">
-        <f t="shared" si="17"/>
         <v>-82077.349999999627</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A81" s="7" t="s">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A99" s="7" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A100" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D100" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A101" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A102" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A103" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A104" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A105" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A106" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A108" s="7" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A82" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B83" s="1" t="s">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A109" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B110" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C83" s="1" t="s">
+      <c r="C110" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A84" t="s">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A111" t="s">
         <v>73</v>
       </c>
-      <c r="B84" s="6">
-        <f>INDEX(B2:B52,MATCH($B$87,$A$2:$A$52,0))</f>
+      <c r="B111" s="6">
+        <f>INDEX($B$2:$B$52,MATCH($B$114,$A$2:$A$52,0))</f>
         <v>356640100</v>
       </c>
-      <c r="C84" s="6">
-        <f>INDEX(C2:C52,MATCH($B$87,$A$2:$A$52,0))</f>
+      <c r="C111" s="6">
+        <f>INDEX($C$2:$C$52,MATCH($B$114,$A$2:$A$52,0))</f>
         <v>341243679.13</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A85" t="s">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A112" t="s">
         <v>74</v>
       </c>
-      <c r="B85" s="6">
-        <f>INDEX($G$2:$G$52,MATCH($B$87,$A$2:$A$52,0))</f>
+      <c r="B112" s="6">
+        <f>INDEX($G$2:$G$52,MATCH($B$114,$A$2:$A$52,0))</f>
         <v>382685200</v>
       </c>
-      <c r="C85" s="6">
-        <f>INDEX(H2:H52,MATCH($B$87,$A$2:$A$52,0))</f>
+      <c r="C112" s="6">
+        <f>INDEX(H2:H52,MATCH($B$114,$A$2:$A$52,0))</f>
         <v>346340810.81999999</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A86" t="s">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A113" t="s">
         <v>75</v>
       </c>
-      <c r="B86" s="6">
-        <f>INDEX($L$2:$L$52,MATCH($B$87,$A$2:$A$52,0))</f>
+      <c r="B113" s="6">
+        <f>INDEX($L$2:$L$52,MATCH($B$114,$A$2:$A$52,0))</f>
         <v>376548600</v>
       </c>
-      <c r="C86" s="6">
-        <f>INDEX($M$2:$M$52,MATCH($B$87,$A$2:$A$52,0))</f>
+      <c r="C113" s="6">
+        <f>INDEX($M$2:$M$52,MATCH($B$114,$A$2:$A$52,0))</f>
         <v>355279492.22999901</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B87" t="s">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B114" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A88" s="7" t="s">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A115" s="7" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A89" t="s">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A116" t="s">
         <v>77</v>
       </c>
-      <c r="B89" s="7">
+      <c r="B116" s="7">
         <v>1</v>
       </c>
-      <c r="C89" s="7"/>
-      <c r="D89" s="7">
+      <c r="C116" s="7"/>
+      <c r="D116" s="7">
         <v>2</v>
       </c>
-      <c r="E89" s="7"/>
-      <c r="F89" s="7">
+      <c r="E116" s="7"/>
+      <c r="F116" s="7">
         <v>3</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B90" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="C90" s="8" t="s">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B117" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C117" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="D90" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="E90" s="8" t="s">
+      <c r="D117" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="E117" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="F90" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="G90" s="8" t="s">
+      <c r="F117" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="G117" s="8" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A91" t="s">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A118" t="s">
         <v>73</v>
       </c>
-      <c r="C91" s="5"/>
-      <c r="E91" s="5"/>
-      <c r="G91" s="5"/>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A92" t="s">
+      <c r="C118" s="5"/>
+      <c r="E118" s="5"/>
+      <c r="G118" s="5"/>
+    </row>
+    <row r="119" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A119" t="s">
         <v>74</v>
       </c>
-      <c r="C92" s="5"/>
-      <c r="E92" s="5"/>
-      <c r="G92" s="5"/>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A93" t="s">
+      <c r="C119" s="5"/>
+      <c r="E119" s="5"/>
+      <c r="G119" s="5"/>
+    </row>
+    <row r="120" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A120" t="s">
         <v>75</v>
       </c>
-      <c r="C93" s="5"/>
-      <c r="E93" s="5"/>
-      <c r="G93" s="5"/>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A95" s="7" t="s">
+      <c r="C120" s="5"/>
+      <c r="E120" s="5"/>
+      <c r="G120" s="5"/>
+    </row>
+    <row r="122" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A122" s="7" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A96" t="s">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A123" t="s">
         <v>77</v>
       </c>
-      <c r="B96" s="7">
+      <c r="B123" s="7">
         <v>1</v>
       </c>
-      <c r="C96" s="7"/>
-      <c r="D96" s="7">
+      <c r="C123" s="7"/>
+      <c r="D123" s="7">
         <v>2</v>
       </c>
-      <c r="E96" s="7"/>
-      <c r="F96" s="7">
+      <c r="E123" s="7"/>
+      <c r="F123" s="7">
         <v>3</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B97" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="C97" s="8" t="s">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B124" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C124" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="D97" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="E97" s="8" t="s">
+      <c r="D124" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="E124" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="F97" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="G97" s="8" t="s">
+      <c r="F124" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="G124" s="8" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A98" t="s">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A125" t="s">
         <v>73</v>
       </c>
-      <c r="C98" s="4"/>
-      <c r="E98" s="4"/>
-      <c r="G98" s="4"/>
-      <c r="I98" s="4"/>
-    </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A99" t="s">
+      <c r="C125" s="4"/>
+      <c r="E125" s="4"/>
+      <c r="G125" s="4"/>
+      <c r="I125" s="4"/>
+    </row>
+    <row r="126" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A126" t="s">
         <v>74</v>
       </c>
-      <c r="C99" s="4"/>
-      <c r="E99" s="4"/>
-      <c r="G99" s="4"/>
-      <c r="I99" s="4"/>
-    </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A100" t="s">
+      <c r="C126" s="4"/>
+      <c r="E126" s="4"/>
+      <c r="G126" s="4"/>
+      <c r="I126" s="4"/>
+    </row>
+    <row r="127" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A127" t="s">
         <v>75</v>
       </c>
-      <c r="C100" s="4"/>
-      <c r="E100" s="4"/>
-      <c r="G100" s="4"/>
-      <c r="I100" s="4"/>
+      <c r="C127" s="4"/>
+      <c r="E127" s="4"/>
+      <c r="G127" s="4"/>
+      <c r="I127" s="4"/>
     </row>
   </sheetData>
-  <dataValidations disablePrompts="1" count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A83" xr:uid="{0ECE0BAD-DC74-4E7B-8842-0609702F3664}">
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A110 B114" xr:uid="{0ECE0BAD-DC74-4E7B-8842-0609702F3664}">
       <formula1>$A$2:$A$52</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B82:B83" xr:uid="{1248789C-8354-428B-8B98-C97B02054C67}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B87" xr:uid="{CFF76C53-869B-4471-95EE-716CACA6C667}">
-      <formula1>$A$2:$A$52</formula1>
-    </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B109:B110" xr:uid="{1248789C-8354-428B-8B98-C97B02054C67}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>